<commit_message>
Added to the notes, added materials used to make the H5P activity
</commit_message>
<xml_diff>
--- a/LectureNotes/Regresson2.xlsx
+++ b/LectureNotes/Regresson2.xlsx
@@ -1,37 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS123-CourseMaterials/LectureNotes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293F9464-BE0C-A246-9B18-9641A082562F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8F1528-BFAB-2A46-84B0-658AE3AE30DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="500" windowWidth="28040" windowHeight="16600" xr2:uid="{51CC137C-92FC-E242-A554-1CE799E2E378}"/>
   </bookViews>
   <sheets>
     <sheet name="Linear Regression" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Linear Regression'!$B$25:$B$30</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Linear Regression'!$C$25:$C$30</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'Linear Regression'!$C$25:$C$30</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'Linear Regression'!$D$25:$D$30</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'Linear Regression'!$B$25:$B$30</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'Linear Regression'!$C$25:$C$30</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'Linear Regression'!$D$25:$D$30</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Linear Regression'!$D$25:$D$30</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Linear Regression'!$B$25:$B$30</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Linear Regression'!$C$25:$C$30</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Linear Regression'!$D$25:$D$30</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Linear Regression'!$B$25:$B$30</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Linear Regression'!$C$25:$C$30</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Linear Regression'!$D$25:$D$30</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Linear Regression'!$B$25:$B$30</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -53,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t># Bedrooms</t>
   </si>
@@ -86,6 +69,21 @@
   </si>
   <si>
     <t>Sigmoid</t>
+  </si>
+  <si>
+    <t>Years of Education</t>
+  </si>
+  <si>
+    <t>Exercise 17</t>
+  </si>
+  <si>
+    <t>Exercise 18</t>
+  </si>
+  <si>
+    <t>Life Expectancy</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -653,24 +651,24 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Linear Regression'!$B$25:$B$30</c:f>
+              <c:f>'Linear Regression'!$B$31:$B$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.5</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.5</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>15</c:v>
@@ -680,7 +678,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Linear Regression'!$C$25:$C$30</c:f>
+              <c:f>'Linear Regression'!$C$31:$C$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -688,13 +686,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -755,24 +753,24 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Linear Regression'!$B$25:$B$30</c:f>
+              <c:f>'Linear Regression'!$B$31:$B$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.5</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.5</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>15</c:v>
@@ -782,23 +780,11 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Linear Regression'!$D$25:$D$30</c:f>
+              <c:f>'Linear Regression'!$D$31:$D$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.88079707797788231</c:v>
-                </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99330714907571527</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.99752737684336534</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.99849881774326299</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>0.99992515377248947</c:v>
                 </c:pt>
                 <c:pt idx="5">
@@ -1009,11 +995,968 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="19350000"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Linear Regression'!$C$57</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Life Expectancy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Linear Regression'!$B$58:$B$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Linear Regression'!$C$58:$C$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-72D5-3C47-B4F1-AB68B35A2D77}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="632237375"/>
+        <c:axId val="578759215"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="632237375"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="20"/>
+          <c:min val="5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Years of Education</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="578759215"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="578759215"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="50"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Life</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Expectancy</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="632237375"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Linear Regression'!$C$78</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Life Expectancy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Linear Regression'!$B$79:$B$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Linear Regression'!$C$79:$C$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D71F-0B43-A6C4-56CBB0DA0EAA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="561076207"/>
+        <c:axId val="585762575"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="561076207"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="25"/>
+          <c:min val="5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Years of Education</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="585762575"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="585762575"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="50"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Life Expectancy</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="561076207"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
@@ -1143,6 +2086,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1660,6 +2683,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2217,13 +4272,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>781050</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>120650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2249,13 +4304,85 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A181E39-1CA0-E653-26F7-BB53A52148C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>817562</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>793749</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E2F32AD-8FF3-6458-C105-1326E5ADC91C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2293,7 +4420,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2399,7 +4526,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2541,7 +4668,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2549,10 +4676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5953DE01-F5C0-5341-89B2-214DEB2450BC}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2647,7 +4774,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:6">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -2661,7 +4788,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="22">
+    <row r="25" spans="1:6" ht="16" customHeight="1">
       <c r="A25" s="3">
         <v>58</v>
       </c>
@@ -2676,86 +4803,348 @@
         <v>0.88079707797788231</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="22">
+    <row r="26" spans="1:6">
       <c r="A26" s="3">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="B26" s="3">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
       </c>
-      <c r="D26" s="4">
-        <f>1/(1+EXP(-B26))</f>
-        <v>0.99330714907571527</v>
-      </c>
+      <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="22">
+    <row r="27" spans="1:6" ht="16" customHeight="1">
       <c r="A27" s="3">
-        <v>215</v>
+        <v>101</v>
       </c>
       <c r="B27" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C27" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" s="4">
         <f>1/(1+EXP(-B27))</f>
-        <v>0.99752737684336534</v>
+        <v>0.99330714907571527</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="22">
+    <row r="28" spans="1:6" ht="16" customHeight="1">
       <c r="A28" s="3">
-        <v>103</v>
+        <v>215</v>
       </c>
       <c r="B28" s="3">
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="C28" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" s="4">
         <f>1/(1+EXP(-B28))</f>
-        <v>0.99849881774326299</v>
+        <v>0.99752737684336534</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="22">
+    <row r="29" spans="1:6" ht="16" customHeight="1">
       <c r="A29" s="3">
-        <v>41</v>
+        <v>103</v>
       </c>
       <c r="B29" s="3">
-        <v>9.5</v>
+        <v>6.5</v>
       </c>
       <c r="C29" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" s="4">
         <f>1/(1+EXP(-B29))</f>
-        <v>0.99992515377248947</v>
+        <v>0.99849881774326299</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="22">
+    <row r="30" spans="1:6">
       <c r="A30" s="3">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="B30" s="3">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C30" s="3">
         <v>1</v>
       </c>
-      <c r="D30" s="4">
-        <f>1/(1+EXP(-B30))</f>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" ht="22" customHeight="1">
+      <c r="A31" s="3">
+        <v>172</v>
+      </c>
+      <c r="B31" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="F31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="22">
+      <c r="A32" s="3">
+        <v>41</v>
+      </c>
+      <c r="B32" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="C32" s="3">
+        <v>1</v>
+      </c>
+      <c r="D32" s="4">
+        <f>1/(1+EXP(-B32))</f>
+        <v>0.99992515377248947</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="22" customHeight="1">
+      <c r="A33" s="3">
+        <v>104</v>
+      </c>
+      <c r="B33" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="C33" s="3">
+        <v>1</v>
+      </c>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" ht="22" customHeight="1">
+      <c r="A34" s="3">
+        <v>201</v>
+      </c>
+      <c r="B34" s="3">
+        <v>12</v>
+      </c>
+      <c r="C34" s="3">
+        <v>1</v>
+      </c>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" ht="22" customHeight="1">
+      <c r="A35" s="3">
+        <v>198</v>
+      </c>
+      <c r="B35" s="3">
+        <v>13</v>
+      </c>
+      <c r="C35" s="3">
+        <v>1</v>
+      </c>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" ht="22">
+      <c r="A36" s="3">
+        <v>24</v>
+      </c>
+      <c r="B36" s="3">
+        <v>15</v>
+      </c>
+      <c r="C36" s="3">
+        <v>1</v>
+      </c>
+      <c r="D36" s="4">
+        <f>1/(1+EXP(-B36))</f>
         <v>0.99999969409777301</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3">
+      <c r="B56" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3">
+      <c r="B57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3">
+      <c r="B58">
+        <v>8</v>
+      </c>
+      <c r="C58">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3">
+      <c r="B59">
+        <v>12</v>
+      </c>
+      <c r="C59">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3">
+      <c r="B60">
+        <v>18</v>
+      </c>
+      <c r="C60">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3">
+      <c r="B77" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3">
+      <c r="B78" t="s">
+        <v>11</v>
+      </c>
+      <c r="C78" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3">
+      <c r="B79">
+        <v>8</v>
+      </c>
+      <c r="C79">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3">
+      <c r="B80">
+        <v>9</v>
+      </c>
+      <c r="C80">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3">
+      <c r="B81">
+        <v>10</v>
+      </c>
+      <c r="C81">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3">
+      <c r="B82">
+        <v>10</v>
+      </c>
+      <c r="C82">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3">
+      <c r="B83">
+        <v>11</v>
+      </c>
+      <c r="C83">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3">
+      <c r="B84">
+        <v>12</v>
+      </c>
+      <c r="C84">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3">
+      <c r="B85">
+        <v>12</v>
+      </c>
+      <c r="C85">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3">
+      <c r="B86">
+        <v>12</v>
+      </c>
+      <c r="C86">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3">
+      <c r="B87">
+        <v>13</v>
+      </c>
+      <c r="C87">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3">
+      <c r="B88">
+        <v>14</v>
+      </c>
+      <c r="C88">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3">
+      <c r="B89">
+        <v>16</v>
+      </c>
+      <c r="C89">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3">
+      <c r="B90">
+        <v>16</v>
+      </c>
+      <c r="C90">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3">
+      <c r="B91">
+        <v>16</v>
+      </c>
+      <c r="C91">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3">
+      <c r="B92">
+        <v>18</v>
+      </c>
+      <c r="C92">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3">
+      <c r="B93">
+        <v>20</v>
+      </c>
+      <c r="C93">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3">
+      <c r="B94">
+        <v>20</v>
+      </c>
+      <c r="C94">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3">
+      <c r="B95">
+        <v>22</v>
+      </c>
+      <c r="C95">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A25:D30">
-    <sortCondition ref="B25:B30"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A25:D36">
+    <sortCondition ref="B25:B36"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>